<commit_message>
Fixing issues flagged by HQ
</commit_message>
<xml_diff>
--- a/input/aggregation/Data aggregation plan_IDP Site level.xlsx
+++ b/input/aggregation/Data aggregation plan_IDP Site level.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/assil_benamor_reach-initiative_org/Documents/DSA 2021/SOM2103_DSA_21/input/aggregation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_C87D47ADE16EF33665591AC07564BBB43869FA47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{304FA4AE-F8D3-7841-843E-135EE9B1A43E}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_C87D47ADE16EF33665591AC07564BBB43869FA47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF7E83ED-09BF-A14B-983A-4B9E65748343}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="760" windowWidth="29260" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="760" windowWidth="29240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA2021" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="458">
   <si>
     <t>type</t>
   </si>
@@ -1795,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="84" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1805,9 +1805,9 @@
     <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="36.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="58.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.33203125" customWidth="1"/>
@@ -5007,12 +5007,6 @@
       </c>
       <c r="G151" t="s">
         <v>14</v>
-      </c>
-      <c r="I151" t="s">
-        <v>30</v>
-      </c>
-      <c r="J151" t="s">
-        <v>366</v>
       </c>
       <c r="K151" t="s">
         <v>30</v>
@@ -5758,6 +5752,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A559C4740925E445AF0B2B750D1B7473" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="906bf6171cc09e52267921fda83b0e92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e" xmlns:ns4="bd40c1a4-aba5-4c6e-9265-7d967b595228" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b40f89ec4c18827ee4e1ba452517ca9" ns3:_="" ns4:_="">
     <xsd:import namespace="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e"/>
@@ -5968,33 +5971,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F039EA79-C75E-4167-9F5D-19D8FED03CCD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="bd40c1a4-aba5-4c6e-9265-7d967b595228"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5712A7AE-99C5-4925-8527-6997984931DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33346E7D-F5E9-41AF-BEE5-4755AF2DCFF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6011,12 +6013,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5712A7AE-99C5-4925-8527-6997984931DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
district / regional data merge
</commit_message>
<xml_diff>
--- a/input/aggregation/Data aggregation plan_IDP Site level.xlsx
+++ b/input/aggregation/Data aggregation plan_IDP Site level.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/assil_benamor_reach-initiative_org/Documents/DSA 2021/SOM2103_DSA_21/input/aggregation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_C87D47ADE16EF33665591AC07564BBB43869FA47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF7E83ED-09BF-A14B-983A-4B9E65748343}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_C87D47ADE16EF33665591AC07564BBB43869FA47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042C02FE-5B1C-4B40-99CA-B0BC0779BC2C}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="760" windowWidth="29240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="31160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA2021" sheetId="5" r:id="rId1"/>
@@ -1795,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5752,15 +5752,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A559C4740925E445AF0B2B750D1B7473" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="906bf6171cc09e52267921fda83b0e92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e" xmlns:ns4="bd40c1a4-aba5-4c6e-9265-7d967b595228" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b40f89ec4c18827ee4e1ba452517ca9" ns3:_="" ns4:_="">
     <xsd:import namespace="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e"/>
@@ -5971,32 +5962,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F039EA79-C75E-4167-9F5D-19D8FED03CCD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="bd40c1a4-aba5-4c6e-9265-7d967b595228"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="3c03b9d1-50a6-43a4-ac1d-3b3601202a1e"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5712A7AE-99C5-4925-8527-6997984931DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33346E7D-F5E9-41AF-BEE5-4755AF2DCFF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6013,4 +6005,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5712A7AE-99C5-4925-8527-6997984931DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>